<commit_message>
2201213 c# project update
최종 수정, PPT, 회의록 추가
</commit_message>
<xml_diff>
--- a/C#/개발정보_ER.xlsx
+++ b/C#/개발정보_ER.xlsx
@@ -528,18 +528,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E47"/>
+  <dimension ref="B3:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.25" customWidth="1"/>
-    <col min="3" max="3" width="16.875" customWidth="1"/>
-    <col min="4" max="4" width="20.625" customWidth="1"/>
-    <col min="5" max="5" width="15.625" customWidth="1"/>
+    <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.375" customWidth="1"/>
     <col min="12" max="12" width="16.25" customWidth="1"/>
     <col min="13" max="14" width="16.375" customWidth="1"/>
@@ -547,7 +547,7 @@
     <col min="18" max="18" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>23</v>
       </c>
@@ -555,7 +555,7 @@
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="2:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -583,7 +583,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
@@ -597,7 +597,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
@@ -611,7 +611,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>19</v>
       </c>
@@ -625,7 +625,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
@@ -639,7 +639,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
@@ -653,15 +653,6 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="7.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="2:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" ht="7.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" ht="7.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" ht="7.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:E3"/>

</xml_diff>